<commit_message>
add Table 1.4, don't gitignore csv result
</commit_message>
<xml_diff>
--- a/data/target_recipes.xlsx
+++ b/data/target_recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R_projects\projects\taxdata-psl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ADC44E-CCD4-41EF-BB50-97D60C4FB5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCADC72D-F105-4090-A29C-0C583FD23EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="1" activeTab="4" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="irs_downloads" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="510">
   <si>
     <t>table</t>
   </si>
@@ -1476,9 +1476,6 @@
     <t>key_concepts</t>
   </si>
   <si>
-    <t>column_2017</t>
-  </si>
-  <si>
     <t>column_2015</t>
   </si>
   <si>
@@ -1489,9 +1486,6 @@
   </si>
   <si>
     <t>rownum_2021</t>
-  </si>
-  <si>
-    <t>rownum_2017</t>
   </si>
   <si>
     <r>
@@ -1575,12 +1569,6 @@
   </si>
   <si>
     <t>rowtype</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
   </si>
   <si>
     <t>description</t>
@@ -1826,7 +1814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1877,9 +1865,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,7 +1902,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>29773</xdr:rowOff>
     </xdr:to>
@@ -1960,8 +1945,8 @@
       <xdr:rowOff>104528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>464821</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>160021</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>160989</xdr:rowOff>
     </xdr:to>
@@ -2009,8 +1994,8 @@
       <xdr:rowOff>18611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>467603</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>162803</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>121081</xdr:rowOff>
     </xdr:to>
@@ -2054,7 +2039,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>68931</xdr:colOff>
+      <xdr:colOff>373731</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -2103,7 +2088,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>197276</xdr:colOff>
+      <xdr:colOff>502076</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>52988</xdr:rowOff>
     </xdr:to>
@@ -2147,7 +2132,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>297992</xdr:colOff>
+      <xdr:colOff>602792</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>178657</xdr:rowOff>
     </xdr:to>
@@ -2190,8 +2175,8 @@
       <xdr:rowOff>84318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>601981</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>297181</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>58121</xdr:rowOff>
     </xdr:to>
@@ -2234,8 +2219,8 @@
       <xdr:rowOff>137100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>412292</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>107492</xdr:colOff>
       <xdr:row>117</xdr:row>
       <xdr:rowOff>25353</xdr:rowOff>
     </xdr:to>
@@ -2279,7 +2264,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>137</xdr:row>
       <xdr:rowOff>77906</xdr:rowOff>
     </xdr:to>
@@ -2323,7 +2308,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>157</xdr:row>
       <xdr:rowOff>172735</xdr:rowOff>
     </xdr:to>
@@ -2360,13 +2345,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>100390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>110685</xdr:rowOff>
@@ -2404,13 +2389,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>119290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>191550</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>153050</xdr:rowOff>
@@ -2448,13 +2433,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>112078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>376201</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>178273</xdr:rowOff>
@@ -2492,13 +2477,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>49</xdr:col>
+      <xdr:col>48</xdr:col>
       <xdr:colOff>206528</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>68159</xdr:rowOff>
@@ -2536,13 +2521,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
       <xdr:row>136</xdr:row>
       <xdr:rowOff>78430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>478774</xdr:colOff>
       <xdr:row>149</xdr:row>
       <xdr:rowOff>49691</xdr:rowOff>
@@ -2580,13 +2565,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>149</xdr:row>
       <xdr:rowOff>159279</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>44</xdr:col>
       <xdr:colOff>193402</xdr:colOff>
       <xdr:row>167</xdr:row>
       <xdr:rowOff>157575</xdr:rowOff>
@@ -2626,6 +2611,407 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>60775</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>48465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D74B824A-18DD-3E00-6084-E4609E66485C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22860" y="15575280"/>
+          <a:ext cx="8313235" cy="4041345"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>28390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>44432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC05050-A619-47D4-BF18-71881873B40F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15207430"/>
+          <a:ext cx="8054340" cy="4953802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>45721</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>38217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>100927</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C0213E3-C9C6-4440-8DD9-C756E4FECE17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="45721" y="20337897"/>
+          <a:ext cx="11849100" cy="4086070"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>94356</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>83587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18B7DEB-9656-4A3C-863A-73C6292985DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="24688800"/>
+          <a:ext cx="11417676" cy="3924067"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>106999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28018125-CDEE-4E0C-9660-46B48C731F08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28712160"/>
+          <a:ext cx="9471660" cy="4861879"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>784859</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>124559</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04213A0B-C816-14AA-2A3A-8BD35199B626}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8237219" y="15303599"/>
+          <a:ext cx="8260081" cy="4919881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>40683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>359147</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>139059</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DADAD509-D348-40D6-92B9-3B5016B74676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12085320" y="20340363"/>
+          <a:ext cx="15446747" cy="4304616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>67252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>410836</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335FA69A-C448-4548-9A2A-9BCC2BE5B0FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11925300" y="24756052"/>
+          <a:ext cx="13829656" cy="4276148"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>264946</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>106714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>438504</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC479B24-2F46-45FB-B1C1-D746D36A3A92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9759466" y="29184634"/>
+          <a:ext cx="9317558" cy="4762466"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2718,7 +3104,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3787,7 +4173,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -3798,7 +4184,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -3810,7 +4196,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -3818,10 +4204,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -3833,10 +4219,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3844,10 +4230,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -3859,7 +4245,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -3867,10 +4253,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -3882,10 +4268,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4434,37 +4820,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76D7A5D-02D8-4436-AE45-CC0DD5660F86}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -4472,11 +4858,11 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B3" s="2">
         <v>29</v>
@@ -4484,32 +4870,29 @@
       <c r="C3" s="2">
         <v>29</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
@@ -4519,15 +4902,14 @@
       <c r="C6" s="18">
         <v>0</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="18" t="s">
+        <v>138</v>
+      </c>
       <c r="E6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>141</v>
       </c>
@@ -4537,15 +4919,14 @@
       <c r="C7" s="18">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="18" t="s">
+        <v>140</v>
+      </c>
       <c r="E7" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>144</v>
       </c>
@@ -4555,15 +4936,14 @@
       <c r="C8" s="18">
         <v>1000</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="18" t="s">
+        <v>143</v>
+      </c>
       <c r="E8" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>147</v>
       </c>
@@ -4573,11 +4953,10 @@
       <c r="C9" s="18">
         <v>1</v>
       </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="18" t="s">
+        <v>146</v>
+      </c>
       <c r="E9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="18" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4589,37 +4968,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A71DED-1A7D-4276-85EC-7E1941122B27}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
@@ -4627,11 +5006,11 @@
       <c r="C2" s="2">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B3" s="2">
         <v>28</v>
@@ -4639,32 +5018,29 @@
       <c r="C3" s="2">
         <v>28</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
@@ -4674,15 +5050,14 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
       <c r="E6" t="s">
         <v>138</v>
       </c>
-      <c r="F6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>141</v>
       </c>
@@ -4692,15 +5067,14 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
       <c r="E7" t="s">
         <v>140</v>
       </c>
-      <c r="F7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>144</v>
       </c>
@@ -4710,15 +5084,14 @@
       <c r="C8">
         <v>1000</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" t="s">
+        <v>152</v>
+      </c>
       <c r="E8" t="s">
         <v>152</v>
       </c>
-      <c r="F8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>153</v>
       </c>
@@ -4728,12 +5101,11 @@
       <c r="C9">
         <v>1000</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>391</v>
       </c>
@@ -4743,15 +5115,14 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
       <c r="E10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>394</v>
       </c>
@@ -4761,15 +5132,14 @@
       <c r="C11">
         <v>1000</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
       <c r="E11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -4779,15 +5149,14 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
       <c r="E12" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>162</v>
       </c>
@@ -4797,15 +5166,14 @@
       <c r="C13">
         <v>1000</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
       <c r="E13" t="s">
-        <v>161</v>
-      </c>
-      <c r="F13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>165</v>
       </c>
@@ -4815,15 +5183,14 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" t="s">
+        <v>164</v>
+      </c>
       <c r="E14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>168</v>
       </c>
@@ -4833,15 +5200,14 @@
       <c r="C15">
         <v>1000</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" t="s">
+        <v>167</v>
+      </c>
       <c r="E15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>171</v>
       </c>
@@ -4851,15 +5217,14 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" t="s">
+        <v>170</v>
+      </c>
       <c r="E16" t="s">
-        <v>170</v>
-      </c>
-      <c r="F16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>118</v>
       </c>
@@ -4869,15 +5234,14 @@
       <c r="C17">
         <v>1000</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" t="s">
+        <v>149</v>
+      </c>
       <c r="E17" t="s">
-        <v>149</v>
-      </c>
-      <c r="F17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>174</v>
       </c>
@@ -4887,15 +5251,14 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
       <c r="E18" t="s">
-        <v>173</v>
-      </c>
-      <c r="F18" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>124</v>
       </c>
@@ -4905,15 +5268,14 @@
       <c r="C19">
         <v>1000</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" t="s">
+        <v>176</v>
+      </c>
       <c r="E19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>177</v>
       </c>
@@ -4923,15 +5285,14 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
       <c r="E20" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>180</v>
       </c>
@@ -4941,15 +5302,14 @@
       <c r="C21">
         <v>1000</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" t="s">
+        <v>179</v>
+      </c>
       <c r="E21" t="s">
-        <v>179</v>
-      </c>
-      <c r="F21" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>193</v>
       </c>
@@ -4959,14 +5319,14 @@
       <c r="C22">
         <v>1</v>
       </c>
+      <c r="D22" t="s">
+        <v>192</v>
+      </c>
       <c r="E22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -4976,16 +5336,15 @@
       <c r="C23">
         <v>1000</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" t="s">
+      <c r="D23" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>210</v>
       </c>
@@ -4995,16 +5354,15 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" t="s">
+        <v>209</v>
+      </c>
       <c r="E24" t="s">
-        <v>209</v>
-      </c>
-      <c r="F24" t="s">
         <v>206</v>
       </c>
-      <c r="O24" s="2"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>213</v>
       </c>
@@ -5014,14 +5372,14 @@
       <c r="C25">
         <v>1000</v>
       </c>
+      <c r="D25" t="s">
+        <v>212</v>
+      </c>
       <c r="E25" t="s">
-        <v>212</v>
-      </c>
-      <c r="F25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>227</v>
       </c>
@@ -5031,14 +5389,14 @@
       <c r="C26">
         <v>1</v>
       </c>
+      <c r="D26" t="s">
+        <v>226</v>
+      </c>
       <c r="E26" t="s">
-        <v>226</v>
-      </c>
-      <c r="F26" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>230</v>
       </c>
@@ -5048,10 +5406,10 @@
       <c r="C27">
         <v>1000</v>
       </c>
+      <c r="D27" t="s">
+        <v>229</v>
+      </c>
       <c r="E27" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" t="s">
         <v>223</v>
       </c>
     </row>
@@ -5063,13 +5421,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F9713-946D-4B96-B17B-71BE4C427E7B}">
-  <dimension ref="A1:K166"/>
+  <dimension ref="A1:J166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5077,28 +5435,28 @@
     <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
@@ -5106,11 +5464,11 @@
       <c r="C2" s="2">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B3" s="2">
         <v>28</v>
@@ -5118,32 +5476,29 @@
       <c r="C3" s="2">
         <v>28</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -5153,14 +5508,14 @@
       <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>141</v>
       </c>
@@ -5170,14 +5525,14 @@
       <c r="C7">
         <v>1</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>144</v>
       </c>
@@ -5187,14 +5542,14 @@
       <c r="C8">
         <v>1000</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>243</v>
       </c>
@@ -5204,14 +5559,14 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>245</v>
       </c>
@@ -5221,14 +5576,14 @@
       <c r="C10">
         <v>1000</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>247</v>
       </c>
@@ -5238,14 +5593,14 @@
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>249</v>
       </c>
@@ -5255,14 +5610,14 @@
       <c r="C12">
         <v>1000</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>251</v>
       </c>
@@ -5272,14 +5627,14 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>253</v>
       </c>
@@ -5289,14 +5644,14 @@
       <c r="C14">
         <v>1000</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>255</v>
       </c>
@@ -5306,14 +5661,14 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>257</v>
       </c>
@@ -5323,14 +5678,14 @@
       <c r="C16">
         <v>1000</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>259</v>
       </c>
@@ -5340,14 +5695,14 @@
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>261</v>
       </c>
@@ -5357,14 +5712,14 @@
       <c r="C18">
         <v>1000</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>263</v>
       </c>
@@ -5374,14 +5729,14 @@
       <c r="C19">
         <v>1</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>265</v>
       </c>
@@ -5391,14 +5746,14 @@
       <c r="C20">
         <v>1000</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>267</v>
       </c>
@@ -5408,14 +5763,14 @@
       <c r="C21">
         <v>1</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>269</v>
       </c>
@@ -5425,14 +5780,14 @@
       <c r="C22">
         <v>1000</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>271</v>
       </c>
@@ -5442,14 +5797,14 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>273</v>
       </c>
@@ -5459,14 +5814,14 @@
       <c r="C24">
         <v>1000</v>
       </c>
+      <c r="D24" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="E24" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>275</v>
       </c>
@@ -5476,14 +5831,14 @@
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="E25" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>277</v>
       </c>
@@ -5493,14 +5848,14 @@
       <c r="C26">
         <v>1000</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="E26" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>279</v>
       </c>
@@ -5510,14 +5865,14 @@
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="E27" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>281</v>
       </c>
@@ -5527,14 +5882,14 @@
       <c r="C28">
         <v>1000</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="E28" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>283</v>
       </c>
@@ -5544,14 +5899,14 @@
       <c r="C29">
         <v>1</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="E29" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>285</v>
       </c>
@@ -5561,14 +5916,14 @@
       <c r="C30">
         <v>1000</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="E30" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>287</v>
       </c>
@@ -5578,14 +5933,14 @@
       <c r="C31">
         <v>1</v>
       </c>
+      <c r="D31" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>289</v>
       </c>
@@ -5595,14 +5950,14 @@
       <c r="C32">
         <v>1000</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>291</v>
       </c>
@@ -5612,14 +5967,14 @@
       <c r="C33">
         <v>1</v>
       </c>
+      <c r="D33" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>293</v>
       </c>
@@ -5629,14 +5984,14 @@
       <c r="C34">
         <v>1000</v>
       </c>
+      <c r="D34" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="E34" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>295</v>
       </c>
@@ -5646,14 +6001,14 @@
       <c r="C35">
         <v>1</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>297</v>
       </c>
@@ -5663,14 +6018,14 @@
       <c r="C36">
         <v>1000</v>
       </c>
+      <c r="D36" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>299</v>
       </c>
@@ -5680,14 +6035,14 @@
       <c r="C37">
         <v>1</v>
       </c>
+      <c r="D37" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="E37" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>301</v>
       </c>
@@ -5697,14 +6052,14 @@
       <c r="C38">
         <v>1000</v>
       </c>
+      <c r="D38" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="E38" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>303</v>
       </c>
@@ -5714,15 +6069,15 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F39" s="19"/>
-      <c r="G39" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E39" s="19"/>
+      <c r="F39" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>305</v>
       </c>
@@ -5732,15 +6087,15 @@
       <c r="C40">
         <v>1000</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F40" s="19"/>
-      <c r="G40" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E40" s="19"/>
+      <c r="F40" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>307</v>
       </c>
@@ -5750,15 +6105,15 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="19"/>
-      <c r="G41" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E41" s="19"/>
+      <c r="F41" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>309</v>
       </c>
@@ -5768,135 +6123,135 @@
       <c r="C42">
         <v>1000</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F42" s="19"/>
-      <c r="G42" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E42" s="19"/>
+      <c r="F42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>492</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="2" t="s">
+      <c r="D43" s="15"/>
+      <c r="E43" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>497</v>
       </c>
       <c r="C44">
         <v>1000</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="2" t="s">
+      <c r="D44" s="15"/>
+      <c r="E44" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>494</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="2" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>499</v>
       </c>
       <c r="C46">
         <v>1000</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="2" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="2" t="s">
+      <c r="D47" s="15"/>
+      <c r="E47" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>501</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>505</v>
       </c>
       <c r="C48">
         <v>1000</v>
       </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="2" t="s">
+      <c r="D48" s="15"/>
+      <c r="E48" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>502</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>506</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="2" t="s">
+      <c r="D49" s="15"/>
+      <c r="E49" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="C50">
         <v>1000</v>
       </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="2" t="s">
+      <c r="D50" s="15"/>
+      <c r="E50" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>311</v>
       </c>
@@ -5906,14 +6261,14 @@
       <c r="C51">
         <v>1</v>
       </c>
+      <c r="D51" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="E51" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F51" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>313</v>
       </c>
@@ -5923,14 +6278,14 @@
       <c r="C52">
         <v>1000</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="E52" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F52" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>315</v>
       </c>
@@ -5940,14 +6295,14 @@
       <c r="C53">
         <v>1</v>
       </c>
+      <c r="D53" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="E53" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F53" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>317</v>
       </c>
@@ -5957,48 +6312,48 @@
       <c r="C54">
         <v>1000</v>
       </c>
+      <c r="D54" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="E54" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F54" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>320</v>
+      </c>
       <c r="E55" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F55" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C56">
         <v>1000</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>321</v>
+      </c>
       <c r="E56" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F56" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>323</v>
       </c>
@@ -6008,14 +6363,14 @@
       <c r="C57">
         <v>1</v>
       </c>
+      <c r="D57" s="2" t="s">
+        <v>322</v>
+      </c>
       <c r="E57" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F57" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>326</v>
       </c>
@@ -6025,14 +6380,14 @@
       <c r="C58">
         <v>1000</v>
       </c>
+      <c r="D58" s="2" t="s">
+        <v>325</v>
+      </c>
       <c r="E58" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="F58" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>329</v>
       </c>
@@ -6042,14 +6397,14 @@
       <c r="C59">
         <v>1</v>
       </c>
+      <c r="D59" s="2" t="s">
+        <v>328</v>
+      </c>
       <c r="E59" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F59" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>332</v>
       </c>
@@ -6059,14 +6414,14 @@
       <c r="C60">
         <v>1000</v>
       </c>
+      <c r="D60" s="2" t="s">
+        <v>331</v>
+      </c>
       <c r="E60" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F60" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>391</v>
       </c>
@@ -6076,14 +6431,14 @@
       <c r="C61">
         <v>1</v>
       </c>
+      <c r="D61" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="E61" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>394</v>
       </c>
@@ -6093,14 +6448,14 @@
       <c r="C62">
         <v>1000</v>
       </c>
+      <c r="D62" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="E62" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>396</v>
       </c>
@@ -6110,12 +6465,12 @@
       <c r="C63">
         <v>1</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="F63" s="19"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E63" s="19"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>153</v>
       </c>
@@ -6125,42 +6480,42 @@
       <c r="C64">
         <v>1000</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="F64" s="19"/>
-    </row>
-    <row r="65" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E64" s="19"/>
+    </row>
+    <row r="65" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
-      <c r="E65" s="19"/>
-      <c r="F65" s="2" t="s">
+      <c r="D65" s="19"/>
+      <c r="E65" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C66">
         <v>1000</v>
       </c>
-      <c r="E66" s="19"/>
-      <c r="F66" s="2" t="s">
+      <c r="D66" s="19"/>
+      <c r="E66" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>404</v>
       </c>
@@ -6170,14 +6525,14 @@
       <c r="C67">
         <v>1</v>
       </c>
+      <c r="D67" s="2" t="s">
+        <v>399</v>
+      </c>
       <c r="E67" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>407</v>
       </c>
@@ -6187,14 +6542,14 @@
       <c r="C68">
         <v>1000</v>
       </c>
+      <c r="D68" s="2" t="s">
+        <v>400</v>
+      </c>
       <c r="E68" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="F68" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>412</v>
       </c>
@@ -6204,14 +6559,14 @@
       <c r="C69">
         <v>1</v>
       </c>
+      <c r="D69" s="2" t="s">
+        <v>403</v>
+      </c>
       <c r="E69" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>109</v>
       </c>
@@ -6221,438 +6576,438 @@
       <c r="C70">
         <v>1000</v>
       </c>
+      <c r="D70" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="E70" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
-      <c r="K75" s="2"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
-      <c r="K76" s="2"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
-      <c r="K77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J77" s="2"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
-      <c r="K78" s="2"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
-      <c r="K79" s="2"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J79" s="2"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
-      <c r="K80" s="2"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
-      <c r="K81" s="2"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J81" s="2"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
-      <c r="K82" s="2"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
-      <c r="K83" s="2"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J83" s="2"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
-      <c r="K84" s="2"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
-      <c r="K85" s="2"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
-      <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
-      <c r="K87" s="2"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
-      <c r="K88" s="2"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
-      <c r="K89" s="2"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J89" s="2"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
-      <c r="K90" s="2"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J90" s="2"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
-      <c r="K91" s="2"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
-      <c r="K92" s="2"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
-      <c r="K93" s="2"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
-      <c r="K94" s="2"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
-      <c r="K95" s="2"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
-      <c r="K96" s="2"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
-      <c r="K97" s="2"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
-      <c r="K98" s="2"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
-      <c r="K99" s="2"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
-      <c r="K100" s="2"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
-      <c r="K101" s="2"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
-      <c r="K102" s="2"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
-      <c r="K103" s="2"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
-      <c r="K104" s="2"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
-      <c r="K105" s="2"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
-      <c r="K106" s="2"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
-      <c r="K107" s="2"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
-      <c r="K108" s="2"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
-      <c r="K109" s="2"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
-      <c r="K110" s="2"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J110" s="2"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
-      <c r="K111" s="2"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J111" s="2"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
-      <c r="K112" s="2"/>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
-      <c r="K113" s="2"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J113" s="2"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
-      <c r="K114" s="2"/>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
-      <c r="K115" s="2"/>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J115" s="2"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
-      <c r="K116" s="2"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J116" s="2"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
-      <c r="K117" s="2"/>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
-      <c r="K118" s="2"/>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
-      <c r="K119" s="2"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
-      <c r="K120" s="2"/>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
-      <c r="K121" s="2"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
-      <c r="K122" s="2"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
-      <c r="K123" s="2"/>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J123" s="2"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
-      <c r="K124" s="2"/>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J124" s="2"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
-      <c r="K125" s="2"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J125" s="2"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
-      <c r="K126" s="2"/>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J126" s="2"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
-      <c r="K127" s="2"/>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J127" s="2"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
-      <c r="K128" s="2"/>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J128" s="2"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
-      <c r="K129" s="2"/>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J129" s="2"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
-      <c r="K130" s="2"/>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J130" s="2"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
-      <c r="K131" s="2"/>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J131" s="2"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
-      <c r="K132" s="2"/>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J132" s="2"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
-      <c r="K133" s="2"/>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J133" s="2"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
-      <c r="K134" s="2"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J134" s="2"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
-      <c r="K135" s="2"/>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J135" s="2"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
-      <c r="K136" s="2"/>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J136" s="2"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
-      <c r="K137" s="2"/>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J137" s="2"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
-      <c r="K138" s="2"/>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K139" s="2"/>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K140" s="2"/>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K141" s="2"/>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K142" s="2"/>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K143" s="2"/>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K144" s="2"/>
-    </row>
-    <row r="145" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K145" s="2"/>
-    </row>
-    <row r="146" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K146" s="2"/>
-    </row>
-    <row r="147" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K147" s="2"/>
-    </row>
-    <row r="148" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K148" s="2"/>
-    </row>
-    <row r="149" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K149" s="2"/>
-    </row>
-    <row r="150" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K150" s="2"/>
-    </row>
-    <row r="151" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K151" s="2"/>
-    </row>
-    <row r="152" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K152" s="2"/>
-    </row>
-    <row r="153" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K153" s="2"/>
-    </row>
-    <row r="154" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K154" s="2"/>
-    </row>
-    <row r="155" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K155" s="2"/>
-    </row>
-    <row r="156" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K156" s="2"/>
-    </row>
-    <row r="157" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K157" s="2"/>
-    </row>
-    <row r="158" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K158" s="2"/>
-    </row>
-    <row r="159" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K159" s="2"/>
-    </row>
-    <row r="160" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K160" s="2"/>
-    </row>
-    <row r="161" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K161" s="2"/>
-    </row>
-    <row r="162" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K162" s="2"/>
-    </row>
-    <row r="163" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K163" s="2"/>
-    </row>
-    <row r="164" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K164" s="2"/>
-    </row>
-    <row r="165" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K165" s="2"/>
-    </row>
-    <row r="166" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K166" s="2"/>
+      <c r="J138" s="2"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J139" s="2"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J140" s="2"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J141" s="2"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J142" s="2"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J144" s="2"/>
+    </row>
+    <row r="145" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J145" s="2"/>
+    </row>
+    <row r="146" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J146" s="2"/>
+    </row>
+    <row r="147" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J147" s="2"/>
+    </row>
+    <row r="148" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J148" s="2"/>
+    </row>
+    <row r="149" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J149" s="2"/>
+    </row>
+    <row r="150" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J151" s="2"/>
+    </row>
+    <row r="152" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J152" s="2"/>
+    </row>
+    <row r="153" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J154" s="2"/>
+    </row>
+    <row r="155" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J155" s="2"/>
+    </row>
+    <row r="156" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J156" s="2"/>
+    </row>
+    <row r="157" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J157" s="2"/>
+    </row>
+    <row r="158" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J158" s="2"/>
+    </row>
+    <row r="159" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J159" s="2"/>
+    </row>
+    <row r="160" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J160" s="2"/>
+    </row>
+    <row r="161" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J161" s="2"/>
+    </row>
+    <row r="162" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J162" s="2"/>
+    </row>
+    <row r="163" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J163" s="2"/>
+    </row>
+    <row r="164" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J164" s="2"/>
+    </row>
+    <row r="165" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J166" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J8:P74">
-    <sortCondition ref="P8:P74"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I8:O74">
+    <sortCondition ref="O8:O74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6661,40 +7016,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0531E3B2-59F3-4C51-ACDB-98FDFE2EB357}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>466</v>
-      </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -6702,135 +7054,716 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="B3" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>462</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>139</v>
+        <v>420</v>
       </c>
       <c r="C6" s="18">
-        <v>0</v>
-      </c>
-      <c r="D6" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>138</v>
+      </c>
       <c r="E6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>141</v>
+        <v>391</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>142</v>
+        <v>392</v>
       </c>
       <c r="C7" s="18">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="18" t="s">
+        <v>140</v>
+      </c>
       <c r="E7" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>144</v>
+        <v>421</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>145</v>
+        <v>422</v>
       </c>
       <c r="C8" s="18">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="18">
         <v>1000</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="18">
+      <c r="D9" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="18">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>146</v>
-      </c>
+      <c r="D10" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>427</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>435</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C18" s="18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>443</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C22" s="18">
+        <v>1</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C23" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>453</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>455</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C25" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C26" s="18">
+        <v>1</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C27" s="18">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J77" s="2"/>
+    </row>
+    <row r="78" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J79" s="2"/>
+    </row>
+    <row r="80" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J81" s="2"/>
+    </row>
+    <row r="82" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J83" s="2"/>
+    </row>
+    <row r="84" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J89" s="2"/>
+    </row>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J90" s="2"/>
+    </row>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J110" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F11:K32">
+    <sortCondition ref="F11:F32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6839,10 +7772,10 @@
   <dimension ref="A1:F357"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E294" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="A226" sqref="A226:G325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated target recipes file
</commit_message>
<xml_diff>
--- a/data/target_recipes.xlsx
+++ b/data/target_recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R_projects\projects\taxdata-psl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCADC72D-F105-4090-A29C-0C583FD23EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78CC42C-B585-425B-A48D-59E88341CE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="1" activeTab="4" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="irs_downloads" sheetId="2" r:id="rId1"/>
@@ -44,8 +44,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={474262C1-F46E-4541-95C6-66B52C288E8E}</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{474262C1-F46E-4541-95C6-66B52C288E8E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CAUTION: Note different income ranges for taxable in 2021</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="513">
   <si>
     <t>table</t>
   </si>
@@ -1671,9 +1689,6 @@
     <t>Partnership net loss</t>
   </si>
   <si>
-    <t>partnership and scorp split in 2021</t>
-  </si>
-  <si>
     <t>scorpinc</t>
   </si>
   <si>
@@ -1711,13 +1726,25 @@
   </si>
   <si>
     <t>vname</t>
+  </si>
+  <si>
+    <t>rownum_2015_txbl</t>
+  </si>
+  <si>
+    <t>rownum_2021_txbl</t>
+  </si>
+  <si>
+    <t>column_2015_txbl</t>
+  </si>
+  <si>
+    <t>column_2021_txbl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,8 +1775,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1777,6 +1810,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1814,7 +1853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1865,6 +1904,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1897,13 +1943,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>139404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>29773</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1941,13 +1987,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>175261</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>104528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>160021</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>160989</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2620,8 +2666,8 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>60775</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>799915</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>48465</xdr:rowOff>
     </xdr:to>
@@ -2665,7 +2711,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:colOff>518160</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>44432</xdr:rowOff>
     </xdr:to>
@@ -2708,8 +2754,8 @@
       <xdr:rowOff>38217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>100927</xdr:rowOff>
     </xdr:to>
@@ -2752,8 +2798,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>94356</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>18156</xdr:colOff>
       <xdr:row>128</xdr:row>
       <xdr:rowOff>83587</xdr:rowOff>
     </xdr:to>
@@ -2797,7 +2843,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>106999</xdr:rowOff>
     </xdr:to>
@@ -2834,13 +2880,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>784859</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>124559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>297180</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
@@ -2878,13 +2924,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>40683</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>359147</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>139059</xdr:rowOff>
@@ -2922,13 +2968,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
       <xdr:row>107</xdr:row>
       <xdr:rowOff>67252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
+      <xdr:col>39</xdr:col>
       <xdr:colOff>410836</xdr:colOff>
       <xdr:row>130</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -2966,13 +3012,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>264946</xdr:colOff>
       <xdr:row>131</xdr:row>
       <xdr:rowOff>106714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>438504</xdr:colOff>
       <xdr:row>157</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -3813,6 +3859,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Don Boyd" id="{E62C18B2-089C-4ED5-8BED-8CDF099F06B2}" userId="6072f2c289e873cd" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4128,6 +4180,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E1" dT="2024-04-03T13:10:32.98" personId="{E62C18B2-089C-4ED5-8BED-8CDF099F06B2}" id="{474262C1-F46E-4541-95C6-66B52C288E8E}">
+    <text>CAUTION: Note different income ranges for taxable in 2021</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4993BB1E-ED9F-4001-B11A-6394D6D6D19B}">
   <dimension ref="A1:H9"/>
@@ -4820,10 +4880,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76D7A5D-02D8-4436-AE45-CC0DD5660F86}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4836,7 +4899,7 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -4846,9 +4909,14 @@
       <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D1" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>483</v>
       </c>
@@ -4858,9 +4926,14 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>482</v>
       </c>
@@ -4870,11 +4943,16 @@
       <c r="C3" s="2">
         <v>29</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>474</v>
@@ -4889,10 +4967,16 @@
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
@@ -4908,8 +4992,14 @@
       <c r="E6" s="18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F6" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>141</v>
       </c>
@@ -4925,8 +5015,14 @@
       <c r="E7" s="18" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>144</v>
       </c>
@@ -4942,22 +5038,11 @@
       <c r="E8" s="18" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="18">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>146</v>
+      <c r="F8" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4967,11 +5052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A71DED-1A7D-4276-85EC-7E1941122B27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A71DED-1A7D-4276-85EC-7E1941122B27}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4984,7 +5072,7 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -4994,9 +5082,14 @@
       <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D1" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>483</v>
       </c>
@@ -5006,9 +5099,14 @@
       <c r="C2" s="2">
         <v>9</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <v>29</v>
+      </c>
+      <c r="E2" s="20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>482</v>
       </c>
@@ -5018,11 +5116,16 @@
       <c r="C3" s="2">
         <v>28</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="15">
+        <v>29</v>
+      </c>
+      <c r="E3" s="20">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>474</v>
@@ -5037,10 +5140,16 @@
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
@@ -5056,8 +5165,14 @@
       <c r="E6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>141</v>
       </c>
@@ -5073,8 +5188,14 @@
       <c r="E7" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>144</v>
       </c>
@@ -5090,8 +5211,14 @@
       <c r="E8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>153</v>
       </c>
@@ -5104,8 +5231,11 @@
       <c r="D9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>391</v>
       </c>
@@ -5121,8 +5251,14 @@
       <c r="E10" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>394</v>
       </c>
@@ -5138,8 +5274,14 @@
       <c r="E11" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>159</v>
       </c>
@@ -5155,8 +5297,14 @@
       <c r="E12" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>162</v>
       </c>
@@ -5172,8 +5320,14 @@
       <c r="E13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>165</v>
       </c>
@@ -5189,8 +5343,14 @@
       <c r="E14" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>168</v>
       </c>
@@ -5206,8 +5366,14 @@
       <c r="E15" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>171</v>
       </c>
@@ -5221,6 +5387,12 @@
         <v>170</v>
       </c>
       <c r="E16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" t="s">
+        <v>170</v>
+      </c>
+      <c r="G16" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5240,6 +5412,12 @@
       <c r="E17" t="s">
         <v>170</v>
       </c>
+      <c r="F17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
@@ -5257,6 +5435,12 @@
       <c r="E18" t="s">
         <v>149</v>
       </c>
+      <c r="F18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -5274,6 +5458,12 @@
       <c r="E19" t="s">
         <v>173</v>
       </c>
+      <c r="F19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
@@ -5291,6 +5481,12 @@
       <c r="E20" t="s">
         <v>176</v>
       </c>
+      <c r="F20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="21" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
@@ -5308,6 +5504,12 @@
       <c r="E21" t="s">
         <v>150</v>
       </c>
+      <c r="F21" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -5325,6 +5527,12 @@
       <c r="E22" t="s">
         <v>190</v>
       </c>
+      <c r="F22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -5342,6 +5550,12 @@
       <c r="E23" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="F23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -5360,6 +5574,12 @@
       <c r="E24" t="s">
         <v>206</v>
       </c>
+      <c r="F24" t="s">
+        <v>209</v>
+      </c>
+      <c r="G24" t="s">
+        <v>206</v>
+      </c>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -5378,6 +5598,12 @@
       <c r="E25" t="s">
         <v>207</v>
       </c>
+      <c r="F25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G25" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -5395,6 +5621,12 @@
       <c r="E26" t="s">
         <v>222</v>
       </c>
+      <c r="F26" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -5412,10 +5644,17 @@
       <c r="E27" t="s">
         <v>223</v>
       </c>
+      <c r="F27" t="s">
+        <v>229</v>
+      </c>
+      <c r="G27" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5427,7 +5666,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5442,7 +5681,7 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -5452,9 +5691,14 @@
       <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D1" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>483</v>
       </c>
@@ -5464,9 +5708,14 @@
       <c r="C2" s="2">
         <v>9</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="15">
+        <v>29</v>
+      </c>
+      <c r="E2" s="22">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>482</v>
       </c>
@@ -5476,11 +5725,16 @@
       <c r="C3" s="2">
         <v>28</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="15">
+        <v>29</v>
+      </c>
+      <c r="E3" s="22">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>474</v>
@@ -5495,10 +5749,13 @@
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>511</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -5514,8 +5771,14 @@
       <c r="E6" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>141</v>
       </c>
@@ -5531,8 +5794,14 @@
       <c r="E7" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>144</v>
       </c>
@@ -5548,8 +5817,14 @@
       <c r="E8" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>243</v>
       </c>
@@ -5565,8 +5840,14 @@
       <c r="E9" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>245</v>
       </c>
@@ -5582,8 +5863,14 @@
       <c r="E10" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>247</v>
       </c>
@@ -5599,8 +5886,14 @@
       <c r="E11" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>249</v>
       </c>
@@ -5616,8 +5909,14 @@
       <c r="E12" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F12" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>251</v>
       </c>
@@ -5633,8 +5932,14 @@
       <c r="E13" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>253</v>
       </c>
@@ -5650,8 +5955,14 @@
       <c r="E14" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>255</v>
       </c>
@@ -5667,8 +5978,14 @@
       <c r="E15" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>257</v>
       </c>
@@ -5684,8 +6001,14 @@
       <c r="E16" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F16" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>259</v>
       </c>
@@ -5701,8 +6024,14 @@
       <c r="E17" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>261</v>
       </c>
@@ -5718,8 +6047,14 @@
       <c r="E18" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>263</v>
       </c>
@@ -5735,8 +6070,14 @@
       <c r="E19" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>265</v>
       </c>
@@ -5752,8 +6093,14 @@
       <c r="E20" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F20" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>267</v>
       </c>
@@ -5769,8 +6116,14 @@
       <c r="E21" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>269</v>
       </c>
@@ -5786,8 +6139,14 @@
       <c r="E22" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>271</v>
       </c>
@@ -5803,8 +6162,14 @@
       <c r="E23" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>273</v>
       </c>
@@ -5820,8 +6185,14 @@
       <c r="E24" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>275</v>
       </c>
@@ -5837,8 +6208,14 @@
       <c r="E25" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F25" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>277</v>
       </c>
@@ -5854,8 +6231,14 @@
       <c r="E26" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>279</v>
       </c>
@@ -5871,8 +6254,14 @@
       <c r="E27" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>281</v>
       </c>
@@ -5888,8 +6277,14 @@
       <c r="E28" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F28" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>283</v>
       </c>
@@ -5905,8 +6300,14 @@
       <c r="E29" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F29" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>285</v>
       </c>
@@ -5922,8 +6323,14 @@
       <c r="E30" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F30" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>287</v>
       </c>
@@ -5939,8 +6346,14 @@
       <c r="E31" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F31" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>289</v>
       </c>
@@ -5956,8 +6369,14 @@
       <c r="E32" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F32" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>291</v>
       </c>
@@ -5973,8 +6392,14 @@
       <c r="E33" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>293</v>
       </c>
@@ -5990,8 +6415,14 @@
       <c r="E34" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F34" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>295</v>
       </c>
@@ -6007,8 +6438,14 @@
       <c r="E35" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F35" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>297</v>
       </c>
@@ -6024,8 +6461,14 @@
       <c r="E36" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F36" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>299</v>
       </c>
@@ -6041,8 +6484,14 @@
       <c r="E37" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F37" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>301</v>
       </c>
@@ -6058,8 +6507,14 @@
       <c r="E38" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F38" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>303</v>
       </c>
@@ -6073,11 +6528,12 @@
         <v>232</v>
       </c>
       <c r="E39" s="19"/>
-      <c r="F39" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F39" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G39" s="19"/>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>305</v>
       </c>
@@ -6091,11 +6547,12 @@
         <v>233</v>
       </c>
       <c r="E40" s="19"/>
-      <c r="F40" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F40" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>307</v>
       </c>
@@ -6109,11 +6566,12 @@
         <v>234</v>
       </c>
       <c r="E41" s="19"/>
-      <c r="F41" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F41" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>309</v>
       </c>
@@ -6127,11 +6585,12 @@
         <v>235</v>
       </c>
       <c r="E42" s="19"/>
-      <c r="F42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F42" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>488</v>
       </c>
@@ -6145,8 +6604,12 @@
       <c r="E43" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="15"/>
+      <c r="G43" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>489</v>
       </c>
@@ -6160,8 +6623,12 @@
       <c r="E44" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F44" s="15"/>
+      <c r="G44" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>490</v>
       </c>
@@ -6175,8 +6642,12 @@
       <c r="E45" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="15"/>
+      <c r="G45" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>491</v>
       </c>
@@ -6190,13 +6661,17 @@
       <c r="E46" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F46" s="15"/>
+      <c r="G46" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -6205,13 +6680,17 @@
       <c r="E47" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F47" s="15"/>
+      <c r="G47" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C48">
         <v>1000</v>
@@ -6220,13 +6699,17 @@
       <c r="E48" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F48" s="15"/>
+      <c r="G48" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6235,13 +6718,17 @@
       <c r="E49" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="15"/>
+      <c r="G49" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C50">
         <v>1000</v>
@@ -6250,8 +6737,12 @@
       <c r="E50" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F50" s="15"/>
+      <c r="G50" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>311</v>
       </c>
@@ -6267,8 +6758,14 @@
       <c r="E51" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>313</v>
       </c>
@@ -6284,8 +6781,14 @@
       <c r="E52" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F52" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>315</v>
       </c>
@@ -6301,8 +6804,14 @@
       <c r="E53" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>317</v>
       </c>
@@ -6318,8 +6827,14 @@
       <c r="E54" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F54" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>485</v>
       </c>
@@ -6335,8 +6850,14 @@
       <c r="E55" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F55" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>484</v>
       </c>
@@ -6352,8 +6873,14 @@
       <c r="E56" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F56" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>323</v>
       </c>
@@ -6369,8 +6896,14 @@
       <c r="E57" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F57" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>326</v>
       </c>
@@ -6386,8 +6919,14 @@
       <c r="E58" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F58" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>329</v>
       </c>
@@ -6403,8 +6942,14 @@
       <c r="E59" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F59" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>332</v>
       </c>
@@ -6420,8 +6965,14 @@
       <c r="E60" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F60" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>391</v>
       </c>
@@ -6437,8 +6988,14 @@
       <c r="E61" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>394</v>
       </c>
@@ -6454,8 +7011,14 @@
       <c r="E62" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>396</v>
       </c>
@@ -6469,8 +7032,12 @@
         <v>388</v>
       </c>
       <c r="E63" s="19"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G63" s="19"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>153</v>
       </c>
@@ -6484,13 +7051,17 @@
         <v>389</v>
       </c>
       <c r="E64" s="19"/>
+      <c r="F64" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -6499,13 +7070,17 @@
       <c r="E65" s="2" t="s">
         <v>388</v>
       </c>
+      <c r="F65" s="19"/>
+      <c r="G65" s="2" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C66">
         <v>1000</v>
@@ -6514,6 +7089,10 @@
       <c r="E66" s="2" t="s">
         <v>389</v>
       </c>
+      <c r="F66" s="19"/>
+      <c r="G66" s="2" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="67" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
@@ -6531,6 +7110,12 @@
       <c r="E67" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="F67" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
@@ -6548,6 +7133,12 @@
       <c r="E68" s="2" t="s">
         <v>400</v>
       </c>
+      <c r="F68" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
@@ -6565,6 +7156,12 @@
       <c r="E69" s="2" t="s">
         <v>403</v>
       </c>
+      <c r="F69" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="70" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
@@ -6580,6 +7177,12 @@
         <v>406</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>406</v>
       </c>
     </row>
@@ -7016,10 +7619,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0531E3B2-59F3-4C51-ACDB-98FDFE2EB357}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7027,12 +7633,12 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>473</v>
       </c>
@@ -7042,9 +7648,14 @@
       <c r="C1" s="16" t="s">
         <v>465</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D1" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>483</v>
       </c>
@@ -7054,9 +7665,14 @@
       <c r="C2" s="2">
         <v>10</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D2" s="15">
+        <v>33</v>
+      </c>
+      <c r="E2" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>482</v>
       </c>
@@ -7066,11 +7682,16 @@
       <c r="C3" s="2">
         <v>32</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="15">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>474</v>
@@ -7085,10 +7706,16 @@
         <v>463</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>69</v>
       </c>
@@ -7104,8 +7731,14 @@
       <c r="E6" s="18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F6" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>391</v>
       </c>
@@ -7121,8 +7754,14 @@
       <c r="E7" s="18" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>421</v>
       </c>
@@ -7138,8 +7777,14 @@
       <c r="E8" s="18" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F8" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>423</v>
       </c>
@@ -7155,8 +7800,14 @@
       <c r="E9" s="18" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F9" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>425</v>
       </c>
@@ -7172,8 +7823,14 @@
       <c r="E10" s="18" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>427</v>
       </c>
@@ -7189,9 +7846,15 @@
       <c r="E11" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F11" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>429</v>
       </c>
@@ -7207,9 +7870,15 @@
       <c r="E12" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F12" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>431</v>
       </c>
@@ -7225,9 +7894,15 @@
       <c r="E13" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F13" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>433</v>
       </c>
@@ -7243,9 +7918,15 @@
       <c r="E14" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>435</v>
       </c>
@@ -7261,9 +7942,15 @@
       <c r="E15" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F15" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>437</v>
       </c>
@@ -7279,9 +7966,15 @@
       <c r="E16" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>439</v>
       </c>
@@ -7297,8 +7990,14 @@
       <c r="E17" s="18" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F17" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>441</v>
       </c>
@@ -7314,8 +8013,14 @@
       <c r="E18" s="18" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>443</v>
       </c>
@@ -7331,8 +8036,14 @@
       <c r="E19" s="18" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F19" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>445</v>
       </c>
@@ -7348,8 +8059,14 @@
       <c r="E20" s="18" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F20" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>447</v>
       </c>
@@ -7365,8 +8082,14 @@
       <c r="E21" s="18" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>449</v>
       </c>
@@ -7382,8 +8105,14 @@
       <c r="E22" s="18" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F22" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>451</v>
       </c>
@@ -7399,8 +8128,14 @@
       <c r="E23" s="18" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F23" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>453</v>
       </c>
@@ -7416,8 +8151,14 @@
       <c r="E24" s="18" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F24" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>455</v>
       </c>
@@ -7433,8 +8174,14 @@
       <c r="E25" s="18" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F25" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>457</v>
       </c>
@@ -7450,8 +8197,14 @@
       <c r="E26" s="18" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F26" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>459</v>
       </c>
@@ -7467,300 +8220,306 @@
       <c r="E27" s="18" t="s">
         <v>362</v>
       </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F27" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="3"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="3"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="3"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="3"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="3"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="3"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="3"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="3"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
       <c r="B36" s="3"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
       <c r="B37" s="3"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J82" s="2"/>
-    </row>
-    <row r="83" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J89" s="2"/>
-    </row>
-    <row r="90" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J90" s="2"/>
-    </row>
-    <row r="91" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J103" s="2"/>
-    </row>
-    <row r="104" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J105" s="2"/>
-    </row>
-    <row r="106" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J108" s="2"/>
-    </row>
-    <row r="109" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J109" s="2"/>
-    </row>
-    <row r="110" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J110" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L87" s="2"/>
+    </row>
+    <row r="88" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L89" s="2"/>
+    </row>
+    <row r="90" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L93" s="2"/>
+    </row>
+    <row r="94" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L95" s="2"/>
+    </row>
+    <row r="96" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L98" s="2"/>
+    </row>
+    <row r="99" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L99" s="2"/>
+    </row>
+    <row r="100" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L101" s="2"/>
+    </row>
+    <row r="102" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L103" s="2"/>
+    </row>
+    <row r="104" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L104" s="2"/>
+    </row>
+    <row r="105" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L105" s="2"/>
+    </row>
+    <row r="106" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L107" s="2"/>
+    </row>
+    <row r="108" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L109" s="2"/>
+    </row>
+    <row r="110" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L110" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F11:K32">
-    <sortCondition ref="F11:F32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H11:M32">
+    <sortCondition ref="H11:H32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add taxable returns to data gathering
</commit_message>
<xml_diff>
--- a/data/target_recipes.xlsx
+++ b/data/target_recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R_projects\projects\taxdata-psl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78CC42C-B585-425B-A48D-59E88341CE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EB824E-42DB-4D9F-926C-284B24A0ACB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="irs_downloads" sheetId="2" r:id="rId1"/>
@@ -44,26 +44,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={474262C1-F46E-4541-95C6-66B52C288E8E}</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{474262C1-F46E-4541-95C6-66B52C288E8E}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CAUTION: Note different income ranges for taxable in 2021</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="509">
   <si>
     <t>table</t>
   </si>
@@ -1492,18 +1474,6 @@
   </si>
   <si>
     <t>key_concepts</t>
-  </si>
-  <si>
-    <t>column_2015</t>
-  </si>
-  <si>
-    <t>column_2021</t>
-  </si>
-  <si>
-    <t>rownum_2015</t>
-  </si>
-  <si>
-    <t>rownum_2021</t>
   </si>
   <si>
     <r>
@@ -1728,23 +1698,23 @@
     <t>vname</t>
   </si>
   <si>
-    <t>rownum_2015_txbl</t>
-  </si>
-  <si>
-    <t>rownum_2021_txbl</t>
-  </si>
-  <si>
-    <t>column_2015_txbl</t>
-  </si>
-  <si>
-    <t>column_2021_txbl</t>
+    <t>filers_2015</t>
+  </si>
+  <si>
+    <t>filers_2021</t>
+  </si>
+  <si>
+    <t>taxable_2015</t>
+  </si>
+  <si>
+    <t>taxable_2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1773,12 +1743,6 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1853,7 +1817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1905,9 +1869,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -3860,9 +3821,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Don Boyd" id="{E62C18B2-089C-4ED5-8BED-8CDF099F06B2}" userId="6072f2c289e873cd" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4180,14 +4139,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E1" dT="2024-04-03T13:10:32.98" personId="{E62C18B2-089C-4ED5-8BED-8CDF099F06B2}" id="{474262C1-F46E-4541-95C6-66B52C288E8E}">
-    <text>CAUTION: Note different income ranges for taxable in 2021</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4993BB1E-ED9F-4001-B11A-6394D6D6D19B}">
   <dimension ref="A1:H9"/>
@@ -4233,7 +4184,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -4244,7 +4195,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -4256,7 +4207,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -4264,10 +4215,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -4279,10 +4230,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -4290,10 +4241,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -4305,7 +4256,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -4313,10 +4264,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -4328,10 +4279,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4886,7 +4837,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4899,26 +4850,26 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>464</v>
+        <v>505</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>465</v>
+        <v>506</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -4935,7 +4886,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B3" s="2">
         <v>29</v>
@@ -4952,28 +4903,28 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>512</v>
+      <c r="D5" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>508</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5052,14 +5003,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A71DED-1A7D-4276-85EC-7E1941122B27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A71DED-1A7D-4276-85EC-7E1941122B27}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5072,26 +5023,26 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>464</v>
+        <v>505</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>465</v>
+        <v>506</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>510</v>
+        <v>507</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
@@ -5108,7 +5059,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B3" s="2">
         <v>28</v>
@@ -5125,28 +5076,28 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>512</v>
+      <c r="D5" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>508</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5654,7 +5605,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5662,11 +5612,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160F9713-946D-4B96-B17B-71BE4C427E7B}">
   <dimension ref="A1:J166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5681,26 +5631,26 @@
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>464</v>
+        <v>505</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>465</v>
+        <v>506</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B2" s="2">
         <v>9</v>
@@ -5711,13 +5661,13 @@
       <c r="D2" s="15">
         <v>29</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="21">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B3" s="2">
         <v>28</v>
@@ -5728,34 +5678,37 @@
       <c r="D3" s="15">
         <v>29</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>508</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -5778,7 +5731,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>141</v>
       </c>
@@ -5801,7 +5754,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>144</v>
       </c>
@@ -5824,7 +5777,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>243</v>
       </c>
@@ -5847,7 +5800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>245</v>
       </c>
@@ -5870,7 +5823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>247</v>
       </c>
@@ -5893,7 +5846,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>249</v>
       </c>
@@ -5916,7 +5869,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>251</v>
       </c>
@@ -5939,7 +5892,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>253</v>
       </c>
@@ -5962,7 +5915,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>255</v>
       </c>
@@ -5985,7 +5938,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>257</v>
       </c>
@@ -6592,10 +6545,10 @@
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>488</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -6611,10 +6564,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>493</v>
       </c>
       <c r="C44">
         <v>1000</v>
@@ -6630,10 +6583,10 @@
     </row>
     <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>490</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -6649,10 +6602,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>495</v>
       </c>
       <c r="C46">
         <v>1000</v>
@@ -6668,10 +6621,10 @@
     </row>
     <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -6687,10 +6640,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>496</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>500</v>
       </c>
       <c r="C48">
         <v>1000</v>
@@ -6706,10 +6659,10 @@
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>501</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -6725,10 +6678,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>502</v>
       </c>
       <c r="C50">
         <v>1000</v>
@@ -6836,10 +6789,10 @@
     </row>
     <row r="55" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -6859,10 +6812,10 @@
     </row>
     <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C56">
         <v>1000</v>
@@ -7058,10 +7011,10 @@
     </row>
     <row r="65" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -7077,10 +7030,10 @@
     </row>
     <row r="66" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C66">
         <v>1000</v>
@@ -7625,7 +7578,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:E3"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7638,26 +7591,26 @@
     <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>464</v>
+        <v>505</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>465</v>
+        <v>506</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -7674,7 +7627,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B3" s="2">
         <v>32</v>
@@ -7691,28 +7644,28 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>512</v>
+      <c r="D5" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>508</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>